<commit_message>
Finished QA with pre-processing
</commit_message>
<xml_diff>
--- a/dataset/QAA/QAA.xlsx
+++ b/dataset/QAA/QAA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Desktop\HAI\Coursework_1\dataset\QAA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Desktop\HAI\Coursework_1\hai\dataset\QAA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0BB8962-3194-46FE-9FF4-15BC10E3C9D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0B8B51B-F65B-47DA-A2A8-8DDC4327FC75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5424" yWindow="1476" windowWidth="17280" windowHeight="9024" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5424" yWindow="1476" windowWidth="17280" windowHeight="9036" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,9 +42,6 @@
     <t>When is the latest checkout?</t>
   </si>
   <si>
-    <t>When does the pool open?</t>
-  </si>
-  <si>
     <t>The pool is open from midday to 10pm.</t>
   </si>
   <si>
@@ -160,6 +157,9 @@
   </si>
   <si>
     <t>You can contact customer service on 07742249022, they will put you through.</t>
+  </si>
+  <si>
+    <t>What time does the pool open?</t>
   </si>
 </sst>
 </file>
@@ -479,18 +479,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
         <v>9</v>
-      </c>
-      <c r="B1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -498,7 +498,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -506,7 +506,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -514,7 +514,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -522,7 +522,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -530,223 +530,223 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" t="s">
         <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" t="s">
         <v>26</v>
-      </c>
-      <c r="B23" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" t="s">
         <v>29</v>
-      </c>
-      <c r="B25" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" t="s">
         <v>36</v>
-      </c>
-      <c r="B29" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31" t="s">
         <v>39</v>
-      </c>
-      <c r="B31" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B32" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
+        <v>42</v>
+      </c>
+      <c r="B33" t="s">
         <v>43</v>
-      </c>
-      <c r="B33" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>